<commit_message>
Updated code and shinyApp
</commit_message>
<xml_diff>
--- a/inst/extdata/Timetable_Master_Management.xlsx
+++ b/inst/extdata/Timetable_Master_Management.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Lo Priore\Documents\MASTER 2.1\Programming\project--G2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Lo Priore\Documents\MASTER 2.1\Programming\project--G2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755ADC61-4994-48FF-B3F6-615D65F9EBFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B4E1CD-C5FF-4BC5-AE1A-9827586C4184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{7D46FA66-D2EE-D643-A8C9-830764CAC309}"/>
   </bookViews>
@@ -102,9 +102,6 @@
     <t>K. Rege</t>
   </si>
   <si>
-    <t>First 7 Weeks</t>
-  </si>
-  <si>
     <t>Genes, Populations and Evolution</t>
   </si>
   <si>
@@ -114,15 +111,9 @@
     <t>Friday</t>
   </si>
   <si>
-    <t>Last 7 Weeks</t>
-  </si>
-  <si>
     <t>M. Christen/K. Rege</t>
   </si>
   <si>
-    <t>Mandatory BA</t>
-  </si>
-  <si>
     <t>Optimization Methods in Management Science</t>
   </si>
   <si>
@@ -549,9 +540,6 @@
     <t>Advanced Programming</t>
   </si>
   <si>
-    <t>BA orientation</t>
-  </si>
-  <si>
     <t>Start</t>
   </si>
   <si>
@@ -562,6 +550,18 @@
   </si>
   <si>
     <t>End_nice</t>
+  </si>
+  <si>
+    <t>First_7_Weeks</t>
+  </si>
+  <si>
+    <t>Last_7_Weeks</t>
+  </si>
+  <si>
+    <t>BA_orientation</t>
+  </si>
+  <si>
+    <t>BA_Mandatory</t>
   </si>
 </sst>
 </file>
@@ -986,7 +986,7 @@
     <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1020,28 +1020,28 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>172</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -1178,7 +1178,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2">
         <v>6</v>
@@ -1339,10 +1339,10 @@
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E9" s="2">
         <v>6</v>
@@ -1377,7 +1377,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
@@ -1418,13 +1418,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="2">
         <v>6</v>
@@ -1459,13 +1459,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E12" s="2">
         <v>6</v>
@@ -1500,13 +1500,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" s="2">
         <v>6</v>
@@ -1544,10 +1544,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E14" s="2">
         <v>6</v>
@@ -1585,10 +1585,10 @@
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E15" s="2">
         <v>6</v>
@@ -1626,10 +1626,10 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2">
         <v>6</v>
@@ -1667,10 +1667,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E17" s="7">
         <v>1.5</v>
@@ -1708,10 +1708,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E18" s="2">
         <v>6</v>
@@ -1749,10 +1749,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E19" s="2">
         <v>6</v>
@@ -1790,7 +1790,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>14</v>
@@ -1831,10 +1831,10 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E21" s="2">
         <v>6</v>
@@ -1872,10 +1872,10 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E22" s="2">
         <v>6</v>
@@ -1913,10 +1913,10 @@
         <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E23" s="2">
         <v>6</v>
@@ -1954,10 +1954,10 @@
         <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E24" s="2">
         <v>6</v>
@@ -1995,10 +1995,10 @@
         <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E25" s="2">
         <v>6</v>
@@ -2036,10 +2036,10 @@
         <v>7</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E26" s="7">
         <v>1.5</v>
@@ -2077,10 +2077,10 @@
         <v>7</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E27" s="2">
         <v>6</v>
@@ -2118,10 +2118,10 @@
         <v>7</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E28" s="2">
         <v>6</v>
@@ -2159,10 +2159,10 @@
         <v>7</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E29" s="2">
         <v>3</v>
@@ -2200,10 +2200,10 @@
         <v>7</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E30" s="2">
         <v>6</v>
@@ -2241,10 +2241,10 @@
         <v>7</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E31" s="2">
         <v>6</v>
@@ -2282,10 +2282,10 @@
         <v>7</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E32" s="2">
         <v>3</v>
@@ -2323,10 +2323,10 @@
         <v>7</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E33" s="2">
         <v>6</v>
@@ -2364,10 +2364,10 @@
         <v>11</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E34" s="2">
         <v>6</v>
@@ -2405,10 +2405,10 @@
         <v>11</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E35" s="2">
         <v>6</v>
@@ -2446,10 +2446,10 @@
         <v>11</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E36" s="2">
         <v>6</v>
@@ -2487,10 +2487,10 @@
         <v>11</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E37" s="2">
         <v>6</v>
@@ -2528,10 +2528,10 @@
         <v>11</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E38" s="2">
         <v>3</v>
@@ -2569,10 +2569,10 @@
         <v>11</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E39" s="2">
         <v>3</v>
@@ -2610,10 +2610,10 @@
         <v>11</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E40" s="2">
         <v>3</v>
@@ -2651,10 +2651,10 @@
         <v>11</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E41" s="2">
         <v>1.5</v>
@@ -2692,10 +2692,10 @@
         <v>11</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E42" s="2">
         <v>6</v>
@@ -2733,10 +2733,10 @@
         <v>11</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E43" s="2">
         <v>6</v>
@@ -2774,10 +2774,10 @@
         <v>11</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E44" s="2">
         <v>1.5</v>
@@ -2815,10 +2815,10 @@
         <v>16</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E45" s="2">
         <v>3</v>
@@ -2856,10 +2856,10 @@
         <v>16</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E46" s="2">
         <v>6</v>
@@ -2897,10 +2897,10 @@
         <v>16</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E47" s="2">
         <v>6</v>
@@ -2938,10 +2938,10 @@
         <v>16</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E48" s="2">
         <v>6</v>
@@ -2979,10 +2979,10 @@
         <v>16</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E49" s="2">
         <v>3</v>
@@ -3020,10 +3020,10 @@
         <v>16</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E50" s="2">
         <v>3</v>
@@ -3061,10 +3061,10 @@
         <v>16</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E51" s="2">
         <v>6</v>
@@ -3102,10 +3102,10 @@
         <v>16</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E52" s="2">
         <v>6</v>
@@ -3140,13 +3140,13 @@
         <v>2</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E53" s="2">
         <v>6</v>
@@ -3181,13 +3181,13 @@
         <v>2</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E54" s="2">
         <v>6</v>
@@ -3222,13 +3222,13 @@
         <v>2</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E55" s="2">
         <v>3</v>
@@ -3263,13 +3263,13 @@
         <v>2</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E56" s="2">
         <v>3</v>
@@ -3304,13 +3304,13 @@
         <v>2</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E57" s="2">
         <v>3</v>
@@ -3345,13 +3345,13 @@
         <v>2</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E58" s="2">
         <v>3</v>
@@ -3386,13 +3386,13 @@
         <v>2</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E59" s="2">
         <v>6</v>
@@ -3427,13 +3427,13 @@
         <v>2</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E60" s="2">
         <v>6</v>
@@ -3468,13 +3468,13 @@
         <v>2</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E61" s="2">
         <v>6</v>
@@ -3512,10 +3512,10 @@
         <v>4</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E62" s="2">
         <v>3</v>
@@ -3553,10 +3553,10 @@
         <v>4</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E63" s="2">
         <v>6</v>
@@ -3594,10 +3594,10 @@
         <v>4</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E64" s="2">
         <v>3</v>
@@ -3635,10 +3635,10 @@
         <v>4</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E65" s="2">
         <v>6</v>
@@ -3676,10 +3676,10 @@
         <v>4</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E66" s="2">
         <v>3</v>
@@ -3717,10 +3717,10 @@
         <v>4</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E67" s="2">
         <v>6</v>
@@ -3758,10 +3758,10 @@
         <v>7</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E68" s="2">
         <v>6</v>
@@ -3799,10 +3799,10 @@
         <v>7</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E69" s="2">
         <v>6</v>
@@ -3840,10 +3840,10 @@
         <v>7</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E70" s="2">
         <v>1.5</v>
@@ -3881,10 +3881,10 @@
         <v>7</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E71" s="2">
         <v>6</v>
@@ -3922,10 +3922,10 @@
         <v>7</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E72" s="10">
         <v>1.5</v>
@@ -3963,10 +3963,10 @@
         <v>7</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E73" s="2">
         <v>3</v>
@@ -4004,10 +4004,10 @@
         <v>7</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E74" s="2">
         <v>3</v>
@@ -4045,10 +4045,10 @@
         <v>7</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E75" s="2">
         <v>6</v>
@@ -4086,10 +4086,10 @@
         <v>11</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E76" s="2">
         <v>3</v>
@@ -4127,10 +4127,10 @@
         <v>11</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E77" s="2">
         <v>6</v>
@@ -4168,10 +4168,10 @@
         <v>11</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E78" s="2">
         <v>6</v>
@@ -4209,10 +4209,10 @@
         <v>11</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E79" s="2">
         <v>3</v>
@@ -4250,10 +4250,10 @@
         <v>11</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E80" s="2">
         <v>3</v>
@@ -4291,10 +4291,10 @@
         <v>11</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E81" s="2">
         <v>6</v>
@@ -4332,10 +4332,10 @@
         <v>11</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E82" s="2">
         <v>6</v>
@@ -4373,10 +4373,10 @@
         <v>11</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E83" s="2">
         <v>6</v>
@@ -4414,10 +4414,10 @@
         <v>11</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E84" s="2">
         <v>6</v>
@@ -4455,10 +4455,10 @@
         <v>11</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E85" s="2">
         <v>3</v>
@@ -4496,10 +4496,10 @@
         <v>16</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E86" s="2">
         <v>6</v>
@@ -4537,10 +4537,10 @@
         <v>16</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E87" s="2">
         <v>6</v>
@@ -4578,10 +4578,10 @@
         <v>16</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E88" s="2">
         <v>6</v>
@@ -4619,10 +4619,10 @@
         <v>16</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E89" s="2">
         <v>3</v>
@@ -4660,10 +4660,10 @@
         <v>16</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E90" s="2">
         <v>3</v>
@@ -4701,10 +4701,10 @@
         <v>16</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E91" s="2">
         <v>6</v>
@@ -4742,10 +4742,10 @@
         <v>16</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E92" s="2">
         <v>3</v>
@@ -4783,10 +4783,10 @@
         <v>16</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E93" s="2">
         <v>3</v>
@@ -4821,13 +4821,13 @@
         <v>3</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E94" s="2">
         <v>6</v>
@@ -4862,13 +4862,13 @@
         <v>3</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E95" s="2">
         <v>3</v>
@@ -4903,13 +4903,13 @@
         <v>3</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E96" s="2">
         <v>6</v>
@@ -4944,13 +4944,13 @@
         <v>3</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E97" s="2">
         <v>3</v>
@@ -4985,13 +4985,13 @@
         <v>3</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E98" s="2">
         <v>3</v>
@@ -5026,13 +5026,13 @@
         <v>3</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E99" s="2">
         <v>6</v>

</xml_diff>

<commit_message>
Corrected mistake in table
</commit_message>
<xml_diff>
--- a/inst/extdata/Timetable_Master_Management.xlsx
+++ b/inst/extdata/Timetable_Master_Management.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Lo Priore\Documents\MASTER 2.1\Programming\project--G2\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Lo Priore\Documents\MASTER 2.1\Programming\project--G2\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B4E1CD-C5FF-4BC5-AE1A-9827586C4184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A92302-2BAD-45B2-B96F-03C327B72614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{7D46FA66-D2EE-D643-A8C9-830764CAC309}"/>
   </bookViews>
@@ -981,12 +981,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEBCED3-0F7A-9D40-B959-B2A6745D0A8C}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1044,7 +1045,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1085,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1167,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1249,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -1290,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -1331,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -1372,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -1495,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -1536,7 +1537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>2</v>
       </c>
@@ -1577,7 +1578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -1618,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>2</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -1782,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>2</v>
       </c>
@@ -1823,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -1864,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>2</v>
       </c>
@@ -1905,7 +1906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>2</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>2</v>
       </c>
@@ -1987,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>2</v>
       </c>
@@ -2028,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>2</v>
       </c>
@@ -2092,13 +2093,13 @@
         <v>1</v>
       </c>
       <c r="H27" s="12">
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="I27" s="12">
         <v>14</v>
       </c>
       <c r="J27" s="3">
-        <v>0.5</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="K27" s="3">
         <v>0.58333333333333337</v>
@@ -2151,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>2</v>
       </c>
@@ -2192,7 +2193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>2</v>
       </c>
@@ -2233,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>2</v>
       </c>
@@ -2274,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>2</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>2</v>
       </c>
@@ -2356,7 +2357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>2</v>
       </c>
@@ -2397,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>2</v>
       </c>
@@ -2438,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>2</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>2</v>
       </c>
@@ -2643,7 +2644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>2</v>
       </c>
@@ -2684,7 +2685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>2</v>
       </c>
@@ -2725,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>2</v>
       </c>
@@ -2766,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>2</v>
       </c>
@@ -2807,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>2</v>
       </c>
@@ -2848,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>2</v>
       </c>
@@ -2889,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>2</v>
       </c>
@@ -2930,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>2</v>
       </c>
@@ -2971,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>2</v>
       </c>
@@ -3094,7 +3095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>2</v>
       </c>
@@ -3135,7 +3136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>2</v>
       </c>
@@ -3176,7 +3177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>2</v>
       </c>
@@ -3340,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>2</v>
       </c>
@@ -3381,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>2</v>
       </c>
@@ -3422,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>2</v>
       </c>
@@ -3463,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>2</v>
       </c>
@@ -3504,7 +3505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>3</v>
       </c>
@@ -3545,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>3</v>
       </c>
@@ -3627,7 +3628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>3</v>
       </c>
@@ -3668,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>3</v>
       </c>
@@ -3709,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>3</v>
       </c>
@@ -3750,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>3</v>
       </c>
@@ -3791,7 +3792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>3</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>3</v>
       </c>
@@ -3914,7 +3915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>3</v>
       </c>
@@ -3955,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>3</v>
       </c>
@@ -3996,7 +3997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>3</v>
       </c>
@@ -4037,7 +4038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>3</v>
       </c>
@@ -4078,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>3</v>
       </c>
@@ -4119,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>3</v>
       </c>
@@ -4160,7 +4161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>3</v>
       </c>
@@ -4201,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>3</v>
       </c>
@@ -4242,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>3</v>
       </c>
@@ -4283,7 +4284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>3</v>
       </c>
@@ -4324,7 +4325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>3</v>
       </c>
@@ -4365,7 +4366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>3</v>
       </c>
@@ -4406,7 +4407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>3</v>
       </c>
@@ -4447,7 +4448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>3</v>
       </c>
@@ -4488,7 +4489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>3</v>
       </c>
@@ -4529,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>3</v>
       </c>
@@ -4570,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>3</v>
       </c>
@@ -4693,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>3</v>
       </c>
@@ -4734,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>3</v>
       </c>
@@ -4775,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>3</v>
       </c>
@@ -4816,7 +4817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>3</v>
       </c>
@@ -4857,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>3</v>
       </c>
@@ -4898,7 +4899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>3</v>
       </c>
@@ -4939,7 +4940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>3</v>
       </c>
@@ -4980,7 +4981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>3</v>
       </c>
@@ -5063,7 +5064,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M99" xr:uid="{FF6BCF00-F687-40BD-9D06-559784E76804}"/>
+  <autoFilter ref="A1:M99" xr:uid="{FF6BCF00-F687-40BD-9D06-559784E76804}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="12.50"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C62" r:id="rId1" tooltip="descriptif" display="https://hecnet.unil.ch/hec/syllabus/descriptif/2670?dyn_lang=fr" xr:uid="{4A23B8D8-680D-4D43-B9FC-6E6A2CB9AC57}"/>
     <hyperlink ref="C63" r:id="rId2" tooltip="descriptif" display="https://hecnet.unil.ch/hec/syllabus/descriptif/2363?dyn_lang=fr" xr:uid="{136EE764-03E9-9D47-867E-753B6A1231DB}"/>

</xml_diff>

<commit_message>
Corrected mistake in Fraud Analytics
</commit_message>
<xml_diff>
--- a/inst/extdata/Timetable_Master_Management.xlsx
+++ b/inst/extdata/Timetable_Master_Management.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Lo Priore\Documents\MASTER 2.1\Programming\project--G2\raw-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Lo Priore\Documents\MASTER 2.1\Programming\project--G2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A92302-2BAD-45B2-B96F-03C327B72614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8222BAD-E751-473D-966A-406732E281CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{7D46FA66-D2EE-D643-A8C9-830764CAC309}"/>
   </bookViews>
@@ -987,7 +987,7 @@
     <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
+      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1127,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>2</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>2</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>2</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>2</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>2</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>2</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>2</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>2</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>2</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>2</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>3</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>3</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>3</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>3</v>
       </c>
       <c r="F76" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G76" s="4">
         <v>1</v>
@@ -4612,7 +4612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>3</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>3</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>3</v>
       </c>
@@ -5065,9 +5065,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M99" xr:uid="{FF6BCF00-F687-40BD-9D06-559784E76804}">
-    <filterColumn colId="7">
+    <filterColumn colId="2">
       <filters>
-        <filter val="12.50"/>
+        <filter val="Fraud and Business Process Analytics"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>